<commit_message>
commiting Extent reprt code
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/AgentSettingsData.xlsx
+++ b/ocms/src/test/resources/TestData/AgentSettingsData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18330" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18720" windowHeight="8040" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Create" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="93">
   <si>
     <t>Modify Reason</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t xml:space="preserve">testQASupervisor8 </t>
+  </si>
+  <si>
+    <t>Chaithra Kanchan</t>
+  </si>
+  <si>
+    <t>Qualified</t>
   </si>
 </sst>
 </file>
@@ -638,8 +644,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +658,7 @@
     <col min="6" max="6" width="33.42578125" customWidth="1"/>
     <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="58.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="75" x14ac:dyDescent="0.25">
@@ -808,7 +815,7 @@
         <v>27</v>
       </c>
       <c r="V2" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>29</v>
@@ -879,7 +886,7 @@
         <v>28</v>
       </c>
       <c r="P3" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>29</v>
@@ -897,7 +904,7 @@
         <v>27</v>
       </c>
       <c r="V3" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>29</v>
@@ -986,7 +993,7 @@
         <v>27</v>
       </c>
       <c r="V4" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>29</v>
@@ -1075,7 +1082,7 @@
         <v>27</v>
       </c>
       <c r="V5" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="W5" s="2" t="s">
         <v>29</v>
@@ -1253,7 +1260,7 @@
         <v>27</v>
       </c>
       <c r="V7" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="W7" s="2" t="s">
         <v>29</v>
@@ -1289,7 +1296,7 @@
   <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,7 +1423,7 @@
         <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -1455,7 +1462,7 @@
         <v>28</v>
       </c>
       <c r="Q2" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>76</v>
@@ -1476,16 +1483,16 @@
         <v>70</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="AB2" t="s">
         <v>26</v>
@@ -1494,7 +1501,7 @@
         <v>29</v>
       </c>
       <c r="AD2" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>33</v>
@@ -1696,8 +1703,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,7 +1820,7 @@
         <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1898,10 +1905,94 @@
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Comitted on 23rd april 20:15
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/AgentSettingsData.xlsx
+++ b/ocms/src/test/resources/TestData/AgentSettingsData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A73500A-6573-48A0-8BB4-8BFAC8AA4398}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18720" windowHeight="3810"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,6 @@
     <sheet name="Invalid" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="95">
   <si>
     <t>Modify Reason</t>
   </si>
@@ -294,12 +294,27 @@
   </si>
   <si>
     <t>Santosh K</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>edi</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -632,28 +647,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="58.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.453125" customWidth="1"/>
+    <col min="14" max="14" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="58.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -742,7 +757,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>74</v>
       </c>
@@ -831,7 +846,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
@@ -920,7 +935,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
@@ -1009,7 +1024,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>74</v>
       </c>
@@ -1098,7 +1113,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -1187,7 +1202,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>81</v>
       </c>
@@ -1283,33 +1298,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="10.453125" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.81640625" customWidth="1"/>
     <col min="17" max="17" width="21" customWidth="1"/>
-    <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="64.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="32.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1404,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>74</v>
       </c>
@@ -1499,7 +1514,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
@@ -1591,7 +1606,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>81</v>
       </c>
@@ -1691,28 +1706,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="64.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1804,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>74</v>
       </c>
@@ -1896,7 +1911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>60</v>
       </c>
@@ -1988,7 +2003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>81</v>
       </c>
@@ -1996,7 +2011,7 @@
         <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -2080,7 +2095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>81</v>
       </c>
@@ -2179,7 +2194,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2187,19 +2202,19 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>41</v>
       </c>
@@ -2225,7 +2240,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>45</v>
       </c>
@@ -2257,25 +2272,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="64.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -2364,7 +2379,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>81</v>
       </c>
@@ -2453,7 +2468,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>81</v>
       </c>
@@ -2542,7 +2557,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
@@ -2631,8 +2646,31 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>